<commit_message>
MDP WIP diensencatalogus met initiele verhaal Jan Willem
</commit_message>
<xml_diff>
--- a/MDT/DienstenCatalogus/Inleesmodel RI overzicht tariefswijziging 2016 dd 31082015.xlsx
+++ b/MDT/DienstenCatalogus/Inleesmodel RI overzicht tariefswijziging 2016 dd 31082015.xlsx
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2117" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2115" uniqueCount="437">
   <si>
     <t>TC_nr</t>
   </si>
@@ -1387,22 +1387,16 @@
     <t>FMB</t>
   </si>
   <si>
-    <t>WettelijkeTaak</t>
-  </si>
-  <si>
     <t>OmschrijvingFMB</t>
   </si>
   <si>
     <t>omschrijving</t>
   </si>
   <si>
-    <t>wettelijkeTaak</t>
-  </si>
-  <si>
-    <t>subtaakNr</t>
-  </si>
-  <si>
-    <t>SubTaakNr</t>
+    <t>subtaakcluster</t>
+  </si>
+  <si>
+    <t>Subtaakcluster</t>
   </si>
 </sst>
 </file>
@@ -7715,7 +7709,7 @@
   <dimension ref="A1:M130"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -7772,16 +7766,14 @@
       <c r="A2" t="s">
         <v>431</v>
       </c>
-      <c r="C2" s="26" t="s">
-        <v>436</v>
-      </c>
+      <c r="C2" s="26"/>
       <c r="D2" s="26" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="E2" s="27"/>
       <c r="F2" s="27"/>
       <c r="G2" s="26" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H2" s="26"/>
       <c r="I2" s="28"/>
@@ -7793,16 +7785,14 @@
       <c r="A3" t="s">
         <v>432</v>
       </c>
-      <c r="C3" s="26" t="s">
-        <v>433</v>
-      </c>
+      <c r="C3" s="26"/>
       <c r="D3" s="26" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="E3" s="27"/>
       <c r="F3" s="27"/>
       <c r="G3" s="26" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H3" s="26"/>
       <c r="I3" s="28"/>
@@ -8042,10 +8032,6 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" t="str">
-        <f t="shared" si="1"/>
-        <v>17100101</v>
-      </c>
       <c r="B10" s="17" t="s">
         <v>344</v>
       </c>
@@ -11481,7 +11467,7 @@
         <v>WT_29</v>
       </c>
       <c r="D100" s="18" t="str">
-        <f t="shared" ref="D100:D131" si="7">LEFT(E100,5)</f>
+        <f t="shared" ref="D100:D119" si="7">LEFT(E100,5)</f>
         <v>29100</v>
       </c>
       <c r="E100">
@@ -12370,7 +12356,7 @@
       </c>
       <c r="I2" s="14">
         <f t="shared" ref="I2:I65" ca="1" si="0">NOW()</f>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -12408,7 +12394,7 @@
       </c>
       <c r="I3" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -12446,7 +12432,7 @@
       </c>
       <c r="I4" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -12484,7 +12470,7 @@
       </c>
       <c r="I5" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -12522,7 +12508,7 @@
       </c>
       <c r="I6" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -12560,7 +12546,7 @@
       </c>
       <c r="I7" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -12598,7 +12584,7 @@
       </c>
       <c r="I8" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -12636,7 +12622,7 @@
       </c>
       <c r="I9" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -12674,7 +12660,7 @@
       </c>
       <c r="I10" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -12712,7 +12698,7 @@
       </c>
       <c r="I11" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -12750,7 +12736,7 @@
       </c>
       <c r="I12" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -12788,7 +12774,7 @@
       </c>
       <c r="I13" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -12826,7 +12812,7 @@
       </c>
       <c r="I14" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -12864,7 +12850,7 @@
       </c>
       <c r="I15" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -12902,7 +12888,7 @@
       </c>
       <c r="I16" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -12940,7 +12926,7 @@
       </c>
       <c r="I17" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -12978,7 +12964,7 @@
       </c>
       <c r="I18" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -13016,7 +13002,7 @@
       </c>
       <c r="I19" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -13054,7 +13040,7 @@
       </c>
       <c r="I20" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
@@ -13092,7 +13078,7 @@
       </c>
       <c r="I21" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
@@ -13130,7 +13116,7 @@
       </c>
       <c r="I22" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
@@ -13168,7 +13154,7 @@
       </c>
       <c r="I23" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
@@ -13206,7 +13192,7 @@
       </c>
       <c r="I24" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
@@ -13244,7 +13230,7 @@
       </c>
       <c r="I25" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
@@ -13282,7 +13268,7 @@
       </c>
       <c r="I26" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
@@ -13320,7 +13306,7 @@
       </c>
       <c r="I27" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
@@ -13358,7 +13344,7 @@
       </c>
       <c r="I28" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
@@ -13396,7 +13382,7 @@
       </c>
       <c r="I29" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
@@ -13434,7 +13420,7 @@
       </c>
       <c r="I30" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
@@ -13472,7 +13458,7 @@
       </c>
       <c r="I31" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
@@ -13510,7 +13496,7 @@
       </c>
       <c r="I32" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
@@ -13548,7 +13534,7 @@
       </c>
       <c r="I33" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
@@ -13586,7 +13572,7 @@
       </c>
       <c r="I34" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
@@ -13624,7 +13610,7 @@
       </c>
       <c r="I35" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
@@ -13662,7 +13648,7 @@
       </c>
       <c r="I36" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
@@ -13700,7 +13686,7 @@
       </c>
       <c r="I37" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
@@ -13738,7 +13724,7 @@
       </c>
       <c r="I38" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
@@ -13776,7 +13762,7 @@
       </c>
       <c r="I39" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
@@ -13814,7 +13800,7 @@
       </c>
       <c r="I40" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
@@ -13852,7 +13838,7 @@
       </c>
       <c r="I41" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
@@ -13890,7 +13876,7 @@
       </c>
       <c r="I42" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
@@ -13928,7 +13914,7 @@
       </c>
       <c r="I43" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
@@ -13966,7 +13952,7 @@
       </c>
       <c r="I44" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
@@ -14004,7 +13990,7 @@
       </c>
       <c r="I45" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
@@ -14042,7 +14028,7 @@
       </c>
       <c r="I46" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
@@ -14080,7 +14066,7 @@
       </c>
       <c r="I47" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
@@ -14118,7 +14104,7 @@
       </c>
       <c r="I48" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
@@ -14156,7 +14142,7 @@
       </c>
       <c r="I49" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
@@ -14194,7 +14180,7 @@
       </c>
       <c r="I50" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
@@ -14232,7 +14218,7 @@
       </c>
       <c r="I51" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
@@ -14270,7 +14256,7 @@
       </c>
       <c r="I52" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
@@ -14308,7 +14294,7 @@
       </c>
       <c r="I53" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
@@ -14346,7 +14332,7 @@
       </c>
       <c r="I54" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
@@ -14384,7 +14370,7 @@
       </c>
       <c r="I55" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
@@ -14422,7 +14408,7 @@
       </c>
       <c r="I56" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
@@ -14460,7 +14446,7 @@
       </c>
       <c r="I57" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
@@ -14498,7 +14484,7 @@
       </c>
       <c r="I58" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
@@ -14536,7 +14522,7 @@
       </c>
       <c r="I59" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
@@ -14574,7 +14560,7 @@
       </c>
       <c r="I60" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
@@ -14612,7 +14598,7 @@
       </c>
       <c r="I61" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
@@ -14650,7 +14636,7 @@
       </c>
       <c r="I62" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
@@ -14688,7 +14674,7 @@
       </c>
       <c r="I63" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
@@ -14726,7 +14712,7 @@
       </c>
       <c r="I64" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
@@ -14764,7 +14750,7 @@
       </c>
       <c r="I65" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
@@ -14802,7 +14788,7 @@
       </c>
       <c r="I66" s="14">
         <f t="shared" ref="I66:I117" ca="1" si="1">NOW()</f>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
@@ -14840,7 +14826,7 @@
       </c>
       <c r="I67" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
@@ -14878,7 +14864,7 @@
       </c>
       <c r="I68" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
@@ -14916,7 +14902,7 @@
       </c>
       <c r="I69" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
@@ -14954,7 +14940,7 @@
       </c>
       <c r="I70" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
@@ -14992,7 +14978,7 @@
       </c>
       <c r="I71" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
@@ -15030,7 +15016,7 @@
       </c>
       <c r="I72" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
@@ -15068,7 +15054,7 @@
       </c>
       <c r="I73" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
@@ -15106,7 +15092,7 @@
       </c>
       <c r="I74" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
@@ -15144,7 +15130,7 @@
       </c>
       <c r="I75" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
@@ -15182,7 +15168,7 @@
       </c>
       <c r="I76" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
@@ -15220,7 +15206,7 @@
       </c>
       <c r="I77" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
@@ -15258,7 +15244,7 @@
       </c>
       <c r="I78" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
@@ -15296,7 +15282,7 @@
       </c>
       <c r="I79" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
@@ -15334,7 +15320,7 @@
       </c>
       <c r="I80" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
@@ -15372,7 +15358,7 @@
       </c>
       <c r="I81" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
@@ -15410,7 +15396,7 @@
       </c>
       <c r="I82" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.3">
@@ -15448,7 +15434,7 @@
       </c>
       <c r="I83" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
@@ -15486,7 +15472,7 @@
       </c>
       <c r="I84" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
@@ -15524,7 +15510,7 @@
       </c>
       <c r="I85" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
@@ -15562,7 +15548,7 @@
       </c>
       <c r="I86" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
@@ -15600,7 +15586,7 @@
       </c>
       <c r="I87" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
@@ -15638,7 +15624,7 @@
       </c>
       <c r="I88" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
@@ -15676,7 +15662,7 @@
       </c>
       <c r="I89" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
@@ -15714,7 +15700,7 @@
       </c>
       <c r="I90" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.3">
@@ -15752,7 +15738,7 @@
       </c>
       <c r="I91" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
@@ -15790,7 +15776,7 @@
       </c>
       <c r="I92" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.3">
@@ -15828,7 +15814,7 @@
       </c>
       <c r="I93" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.3">
@@ -15866,7 +15852,7 @@
       </c>
       <c r="I94" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
@@ -15904,7 +15890,7 @@
       </c>
       <c r="I95" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.3">
@@ -15942,7 +15928,7 @@
       </c>
       <c r="I96" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.3">
@@ -15980,7 +15966,7 @@
       </c>
       <c r="I97" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.3">
@@ -16018,7 +16004,7 @@
       </c>
       <c r="I98" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
@@ -16056,7 +16042,7 @@
       </c>
       <c r="I99" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
@@ -16094,7 +16080,7 @@
       </c>
       <c r="I100" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.3">
@@ -16132,7 +16118,7 @@
       </c>
       <c r="I101" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.3">
@@ -16170,7 +16156,7 @@
       </c>
       <c r="I102" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.3">
@@ -16208,7 +16194,7 @@
       </c>
       <c r="I103" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.3">
@@ -16246,7 +16232,7 @@
       </c>
       <c r="I104" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.3">
@@ -16284,7 +16270,7 @@
       </c>
       <c r="I105" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.3">
@@ -16322,7 +16308,7 @@
       </c>
       <c r="I106" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.3">
@@ -16360,7 +16346,7 @@
       </c>
       <c r="I107" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.3">
@@ -16398,7 +16384,7 @@
       </c>
       <c r="I108" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.3">
@@ -16436,7 +16422,7 @@
       </c>
       <c r="I109" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.3">
@@ -16474,7 +16460,7 @@
       </c>
       <c r="I110" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.3">
@@ -16512,7 +16498,7 @@
       </c>
       <c r="I111" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.3">
@@ -16550,7 +16536,7 @@
       </c>
       <c r="I112" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.3">
@@ -16588,7 +16574,7 @@
       </c>
       <c r="I113" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.3">
@@ -16626,7 +16612,7 @@
       </c>
       <c r="I114" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.3">
@@ -16664,7 +16650,7 @@
       </c>
       <c r="I115" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.3">
@@ -16702,7 +16688,7 @@
       </c>
       <c r="I116" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.3">
@@ -16740,7 +16726,7 @@
       </c>
       <c r="I117" s="14">
         <f t="shared" ca="1" si="1"/>
-        <v>42394.69300821759</v>
+        <v>42396.617647569445</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>